<commit_message>
changed: hash to indexing
</commit_message>
<xml_diff>
--- a/xlsmapper.xlsx
+++ b/xlsmapper.xlsx
@@ -8,19 +8,19 @@
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId4"/>
-    <sheet name="9efca05aa9dbcc9a38cb5ad7589375e" sheetId="2" r:id="rId5"/>
-    <sheet name="806fb77b23d8634ec34b3ef3501108a" sheetId="3" r:id="rId6"/>
-    <sheet name="f2a15aef39aa48c289e31ee5af8773d" sheetId="4" r:id="rId7"/>
-    <sheet name="c750efac7d325aa665708f407d8fbc2" sheetId="5" r:id="rId8"/>
-    <sheet name="8f61ef20650c1716366f7e03533b329" sheetId="6" r:id="rId9"/>
-    <sheet name="866c414e9613636f23fbfffe59110c8" sheetId="7" r:id="rId10"/>
-    <sheet name="8b44d8a9229391491a00fad35330512" sheetId="8" r:id="rId11"/>
-    <sheet name="316eff8ca8b4fad2ccc14b88612d44e" sheetId="9" r:id="rId12"/>
-    <sheet name="a3d727e7f89383623482b9062cd5bdf" sheetId="10" r:id="rId13"/>
-    <sheet name="5e82e759bfb391695af6697ac5b0ef1" sheetId="11" r:id="rId14"/>
-    <sheet name="cea2d265497ee41ef6c56079c613cf1" sheetId="12" r:id="rId15"/>
-    <sheet name="be10686d3f0858d36031bad251051c5" sheetId="13" r:id="rId16"/>
-    <sheet name="579d5971a9cbb83b41d70ea368ed033" sheetId="14" r:id="rId17"/>
+    <sheet name="2" sheetId="2" r:id="rId5"/>
+    <sheet name="3" sheetId="3" r:id="rId6"/>
+    <sheet name="4" sheetId="4" r:id="rId7"/>
+    <sheet name="5" sheetId="5" r:id="rId8"/>
+    <sheet name="6" sheetId="6" r:id="rId9"/>
+    <sheet name="7" sheetId="7" r:id="rId10"/>
+    <sheet name="8" sheetId="8" r:id="rId11"/>
+    <sheet name="9" sheetId="9" r:id="rId12"/>
+    <sheet name="10" sheetId="10" r:id="rId13"/>
+    <sheet name="11" sheetId="11" r:id="rId14"/>
+    <sheet name="12" sheetId="12" r:id="rId15"/>
+    <sheet name="13" sheetId="13" r:id="rId16"/>
+    <sheet name="14" sheetId="14" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -28,83 +28,44 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
-  <si>
-    <t>9efca05aa9dbcc9a38cb5ad7589375e</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="77">
   <si>
     <t>./TestSerializacjiObiektow-Student.csv</t>
   </si>
   <si>
-    <t>806fb77b23d8634ec34b3ef3501108a</t>
-  </si>
-  <si>
     <t>./TestTypes-Student.csv</t>
   </si>
   <si>
-    <t>f2a15aef39aa48c289e31ee5af8773d</t>
-  </si>
-  <si>
     <t>./TestObjectCopies-B.csv</t>
   </si>
   <si>
-    <t>c750efac7d325aa665708f407d8fbc2</t>
-  </si>
-  <si>
     <t>./TestObjectCopies-A.csv</t>
   </si>
   <si>
-    <t>8f61ef20650c1716366f7e03533b329</t>
-  </si>
-  <si>
     <t>./TestCyclicRelations-C.csv</t>
   </si>
   <si>
-    <t>866c414e9613636f23fbfffe59110c8</t>
-  </si>
-  <si>
     <t>./TestCyclicRelations-B.csv</t>
   </si>
   <si>
-    <t>8b44d8a9229391491a00fad35330512</t>
-  </si>
-  <si>
     <t>./TestCyclicRelations-A.csv</t>
   </si>
   <si>
-    <t>316eff8ca8b4fad2ccc14b88612d44e</t>
-  </si>
-  <si>
     <t>./TestLists-Student.csv</t>
   </si>
   <si>
-    <t>a3d727e7f89383623482b9062cd5bdf</t>
-  </si>
-  <si>
     <t>./TestListsObjs-Ocena.csv</t>
   </si>
   <si>
-    <t>5e82e759bfb391695af6697ac5b0ef1</t>
-  </si>
-  <si>
     <t>./TestListsObjs-Student.csv</t>
   </si>
   <si>
-    <t>cea2d265497ee41ef6c56079c613cf1</t>
-  </si>
-  <si>
     <t>./TestDziedziczenia-Student.csv</t>
   </si>
   <si>
-    <t>be10686d3f0858d36031bad251051c5</t>
-  </si>
-  <si>
     <t>./TestKompozycja-Silnik.csv</t>
   </si>
   <si>
-    <t>579d5971a9cbb83b41d70ea368ed033</t>
-  </si>
-  <si>
     <t>./TestKompozycja-Samochod.csv</t>
   </si>
   <si>
@@ -123,7 +84,7 @@
     <t xml:space="preserve"> 18</t>
   </si>
   <si>
-    <t xml:space="preserve"> 6664bcc61fa23</t>
+    <t xml:space="preserve"> 6669da604354f</t>
   </si>
   <si>
     <t xml:space="preserve"> wysokosc</t>
@@ -138,7 +99,7 @@
     <t xml:space="preserve"> 165.75</t>
   </si>
   <si>
-    <t xml:space="preserve"> 6664bcc62500f</t>
+    <t xml:space="preserve"> 6669da60494b6</t>
   </si>
   <si>
     <t>value</t>
@@ -147,10 +108,10 @@
     <t>anything</t>
   </si>
   <si>
-    <t xml:space="preserve"> 6664bcc6281f4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6664bcc6281fb</t>
+    <t xml:space="preserve"> 6669da604d2f0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6669da604d2fb</t>
   </si>
   <si>
     <t>b1@TestObjectCopies\B</t>
@@ -162,37 +123,37 @@
     <t xml:space="preserve"> b3@TestObjectCopies\B</t>
   </si>
   <si>
-    <t>6664bcc6281f4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6664bcc6281ee</t>
+    <t>6669da604d2f0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6669da604d2e7</t>
   </si>
   <si>
     <t>a@TestCyclicRelations\A</t>
   </si>
   <si>
-    <t>6664bcc62eccc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6664bcc62ecd2</t>
+    <t>6669da6057c84</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6669da6057c8d</t>
   </si>
   <si>
     <t>c@TestCyclicRelations\C</t>
   </si>
   <si>
-    <t>6664bcc62ecd2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6664bcc62ecd1</t>
+    <t>6669da6057c8d</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6669da6057c8a</t>
   </si>
   <si>
     <t>b@TestCyclicRelations\B</t>
   </si>
   <si>
-    <t>6664bcc62ecd1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6664bcc62eccc</t>
+    <t>6669da6057c8a</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6669da6057c84</t>
   </si>
   <si>
     <t xml:space="preserve"> ~oceny</t>
@@ -204,7 +165,7 @@
     <t xml:space="preserve"> 2,2,3,1</t>
   </si>
   <si>
-    <t xml:space="preserve"> 6664bcc63af27</t>
+    <t xml:space="preserve"> 6669da6072678</t>
   </si>
   <si>
     <t>ocena</t>
@@ -216,46 +177,46 @@
     <t xml:space="preserve"> 1</t>
   </si>
   <si>
-    <t xml:space="preserve"> 6664bcc63ffcc</t>
+    <t xml:space="preserve"> 6669da60832b0</t>
   </si>
   <si>
     <t xml:space="preserve"> 2</t>
   </si>
   <si>
-    <t xml:space="preserve"> 6664bcc63ffd2</t>
+    <t xml:space="preserve"> 6669da60832b6</t>
   </si>
   <si>
     <t xml:space="preserve"> 3</t>
   </si>
   <si>
-    <t xml:space="preserve"> 6664bcc63ffd5</t>
+    <t xml:space="preserve"> 6669da60832b9</t>
   </si>
   <si>
     <t xml:space="preserve"> 4</t>
   </si>
   <si>
-    <t xml:space="preserve"> 6664bcc63ffd8</t>
+    <t xml:space="preserve"> 6669da60832bc</t>
   </si>
   <si>
     <t xml:space="preserve"> 5</t>
   </si>
   <si>
-    <t xml:space="preserve"> 6664bcc63ffdb</t>
+    <t xml:space="preserve"> 6669da60832bf</t>
   </si>
   <si>
     <t xml:space="preserve"> 6</t>
   </si>
   <si>
-    <t xml:space="preserve"> 6664bcc63ffdf</t>
+    <t xml:space="preserve"> 6669da60832c3</t>
   </si>
   <si>
     <t xml:space="preserve"> ~oceny@TestListsObjs\Ocena</t>
   </si>
   <si>
-    <t xml:space="preserve"> 6664bcc63ffcc,6664bcc63ffd2,6664bcc63ffd5,6664bcc63ffd8,6664bcc63ffdb,6664bcc63ffdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6664bcc63ffc5</t>
+    <t xml:space="preserve"> 6669da60832b0,6669da60832b6,6669da60832b9,6669da60832bc,6669da60832bf,6669da60832c3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6669da60832a6</t>
   </si>
   <si>
     <t>numerIndeksu</t>
@@ -276,7 +237,7 @@
     <t xml:space="preserve"> Ślimak</t>
   </si>
   <si>
-    <t xml:space="preserve"> 6664bcc64a47d</t>
+    <t xml:space="preserve"> 6669da60a0baa</t>
   </si>
   <si>
     <t>moc</t>
@@ -285,7 +246,7 @@
     <t>245KM</t>
   </si>
   <si>
-    <t xml:space="preserve"> 6664bcc64fd42</t>
+    <t xml:space="preserve"> 6669da60ae317</t>
   </si>
   <si>
     <t>model</t>
@@ -297,7 +258,7 @@
     <t>528i</t>
   </si>
   <si>
-    <t xml:space="preserve"> 6664bcc64fd3a</t>
+    <t xml:space="preserve"> 6669da60ae30b</t>
   </si>
 </sst>
 </file>
@@ -645,108 +606,109 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
+    <row r="1" spans="1:2"/>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
         <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -771,13 +733,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -785,10 +747,10 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -796,10 +758,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -807,10 +769,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -818,10 +780,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -829,10 +791,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -840,10 +802,10 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -868,24 +830,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -910,30 +872,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -958,18 +920,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -994,24 +956,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1036,24 +998,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1078,30 +1040,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1126,26 +1088,26 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1170,30 +1132,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1218,18 +1180,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1254,18 +1216,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1290,18 +1252,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1326,24 +1288,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>